<commit_message>
Changes done for remaining KIT testcases
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC15_Verify_MyaccountSection_for_all_Usertype.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC15_Verify_MyaccountSection_for_all_Usertype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B29E5E-C246-4263-8DF2-7BD40DF3351D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED65E395-BA65-431D-B745-561FC8EE8CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="72">
   <si>
     <t>TestCase</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>TC15_Verify_MyaccountSection_for_all_Usertype</t>
+  </si>
+  <si>
+    <t>LoginURL</t>
   </si>
 </sst>
 </file>
@@ -693,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -781,17 +784,15 @@
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
@@ -799,51 +800,51 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
@@ -851,19 +852,19 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>46</v>
@@ -871,22 +872,22 @@
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
@@ -894,13 +895,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -909,13 +910,13 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -923,14 +924,14 @@
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>44</v>
+      <c r="C17" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>44</v>
+      <c r="E17" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -939,13 +940,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -954,13 +955,13 @@
         <v>11</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -969,13 +970,13 @@
         <v>11</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -984,13 +985,13 @@
         <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -999,13 +1000,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1013,14 +1014,14 @@
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>51</v>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>51</v>
+      <c r="E23" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1029,19 +1030,19 @@
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>52</v>
@@ -1049,44 +1050,44 @@
       <c r="D25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3"/>
@@ -1094,69 +1095,69 @@
         <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3"/>
-      <c r="B30" s="4" t="s">
-        <v>15</v>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>18</v>
@@ -1164,22 +1165,22 @@
       <c r="D34" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
-        <v>11</v>
+      <c r="B35" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3"/>
@@ -1187,13 +1188,13 @@
         <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1202,13 +1203,13 @@
         <v>11</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1216,14 +1217,14 @@
       <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>44</v>
+      <c r="C38" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>44</v>
+      <c r="E38" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1232,13 +1233,13 @@
         <v>11</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1247,13 +1248,13 @@
         <v>11</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1262,13 +1263,13 @@
         <v>11</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1277,13 +1278,13 @@
         <v>11</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1292,13 +1293,13 @@
         <v>11</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1306,14 +1307,14 @@
       <c r="B44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>51</v>
+      <c r="C44" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>51</v>
+      <c r="E44" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1322,19 +1323,19 @@
         <v>11</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>52</v>
@@ -1342,44 +1343,44 @@
       <c r="D46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3"/>
@@ -1387,56 +1388,56 @@
         <v>10</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3"/>
-      <c r="B51" s="4" t="s">
-        <v>15</v>
+      <c r="B51" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3"/>
       <c r="B53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>18</v>
@@ -1444,22 +1445,22 @@
       <c r="D54" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3"/>
-      <c r="B55" s="3" t="s">
-        <v>11</v>
+      <c r="B55" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3"/>
@@ -1467,13 +1468,13 @@
         <v>11</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1482,13 +1483,13 @@
         <v>11</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1496,14 +1497,14 @@
       <c r="B58" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>44</v>
+      <c r="C58" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E58" s="5" t="s">
-        <v>44</v>
+      <c r="E58" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1512,13 +1513,13 @@
         <v>11</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1527,13 +1528,13 @@
         <v>11</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1542,13 +1543,13 @@
         <v>11</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1557,13 +1558,13 @@
         <v>11</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1572,13 +1573,13 @@
         <v>11</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1586,14 +1587,14 @@
       <c r="B64" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>51</v>
+      <c r="C64" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>51</v>
+      <c r="E64" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1602,19 +1603,19 @@
         <v>11</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D65" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3"/>
       <c r="B66" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>52</v>
@@ -1622,44 +1623,44 @@
       <c r="D66" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3"/>
       <c r="B67" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3"/>
       <c r="B68" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E68" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3"/>
       <c r="B69" s="3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3"/>
@@ -1667,56 +1668,56 @@
         <v>10</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3"/>
-      <c r="B71" s="4" t="s">
-        <v>15</v>
+      <c r="B71" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3"/>
       <c r="B73" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3"/>
       <c r="B74" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>18</v>
@@ -1724,22 +1725,22 @@
       <c r="D74" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3"/>
-      <c r="B75" s="3" t="s">
-        <v>11</v>
+      <c r="B75" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3"/>
@@ -1747,13 +1748,13 @@
         <v>11</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1762,13 +1763,13 @@
         <v>11</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1776,14 +1777,14 @@
       <c r="B78" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>44</v>
+      <c r="C78" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>44</v>
+      <c r="E78" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1792,13 +1793,13 @@
         <v>11</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1807,13 +1808,13 @@
         <v>11</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1822,13 +1823,13 @@
         <v>11</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1837,13 +1838,13 @@
         <v>11</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1852,13 +1853,13 @@
         <v>11</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1866,14 +1867,14 @@
       <c r="B84" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>51</v>
+      <c r="C84" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>51</v>
+      <c r="E84" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1882,19 +1883,19 @@
         <v>11</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3"/>
       <c r="B86" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>52</v>
@@ -1902,7 +1903,22 @@
       <c r="D86" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E87" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -2191,12 +2207,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2205,7 +2215,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -2402,24 +2412,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2427,7 +2426,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2444,4 +2443,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>